<commit_message>
polished adeverinta de venit
</commit_message>
<xml_diff>
--- a/server/src/main/java/net/guides/springboot2/crud/templates/AdeverintaDeVenit.xlsx
+++ b/server/src/main/java/net/guides/springboot2/crud/templates/AdeverintaDeVenit.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\webapp-spring\server\src\main\java\net\guides\springboot2\crud\templates\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B1EB3D-8F7F-4C2E-808D-2ED21E1EDD17}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="334" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="334"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Tel.:</t>
   </si>
@@ -31,9 +25,6 @@
     <t>Nr. de inregistrare ................... / .........................</t>
   </si>
   <si>
-    <t>si impozite cu retinere la sursa:</t>
-  </si>
-  <si>
     <t>Date informative privind impozitul pe veniturile din salarii:</t>
   </si>
   <si>
@@ -61,12 +52,6 @@
     <t>TOTAL</t>
   </si>
   <si>
-    <t xml:space="preserve">      Prin prezenta se atesta faptul ca dl./dna [nume] domiciliat(a)</t>
-  </si>
-  <si>
-    <t>in [localitate], [adresa], judetul [judet]</t>
-  </si>
-  <si>
     <t>[nume societate]</t>
   </si>
   <si>
@@ -79,12 +64,6 @@
     <t>[cui]</t>
   </si>
   <si>
-    <t>[judet], posesor al BI/CI seria [serie], nr. [nr], CNP [cnp] are calitatea de</t>
-  </si>
-  <si>
-    <t>salariat incepand cu data de dd.mm.yyy si a inregistrat in anul yyy urmatoarele venituri</t>
-  </si>
-  <si>
     <t>Perioada: 01/mm/yyyy - 31/mm/yyyy</t>
   </si>
   <si>
@@ -101,12 +80,15 @@
   </si>
   <si>
     <t>Natura venitului: 07. Venituri din salarii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Prin prezenta se atesta faptul ca dl./dna POPESCU ION-IONUT domiciliat(a) in Bucuresti, Bld.Bulevardul Mic 10, bl. 12, sc. A, sector 7, judetul Bucuresti, posesor al BI/CI seria RX, nr 132456, CNP 1234567890123 are calitatea de salariat incepand cu data de dd.mm.yyy si a inregistrat in anul yyyy urmatoarele venituri si impozite cu retinere la sursa:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0000000000"/>
     <numFmt numFmtId="165" formatCode="????????"/>
@@ -161,7 +143,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color indexed="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -433,6 +414,12 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="justify" wrapText="1"/>
+    </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -443,9 +430,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -454,9 +438,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -596,7 +577,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -648,7 +629,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -842,21 +823,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:N60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -867,166 +848,194 @@
     <col min="4" max="4" width="16" style="13"/>
     <col min="5" max="5" width="14.6640625" style="13" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="11.88671875" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="7" max="7" width="7.33203125" customWidth="1"/>
+    <col min="14" max="14" width="31.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-    </row>
-    <row r="2" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-    </row>
-    <row r="3" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+    </row>
+    <row r="2" spans="1:14" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+    </row>
+    <row r="3" spans="1:14" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-    </row>
-    <row r="4" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+    </row>
+    <row r="4" spans="1:14" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-    </row>
-    <row r="5" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
+      <c r="B4" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+    </row>
+    <row r="5" spans="1:14" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-    </row>
-    <row r="6" spans="1:7" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-    </row>
-    <row r="7" spans="1:7" s="3" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-    </row>
-    <row r="8" spans="1:7" s="3" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-    </row>
-    <row r="9" spans="1:7" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-    </row>
-    <row r="10" spans="1:7" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-    </row>
-    <row r="11" spans="1:7" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-    </row>
-    <row r="12" spans="1:7" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+    </row>
+    <row r="6" spans="1:14" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="35"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+    </row>
+    <row r="7" spans="1:14" s="3" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-    </row>
-    <row r="13" spans="1:7" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+    </row>
+    <row r="8" spans="1:14" s="3" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-    </row>
-    <row r="14" spans="1:7" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="32"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-    </row>
-    <row r="15" spans="1:7" s="13" customFormat="1" ht="10.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+    </row>
+    <row r="9" spans="1:14" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="35"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+    </row>
+    <row r="10" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+    </row>
+    <row r="11" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="29"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
+    </row>
+    <row r="12" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="29"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
+    </row>
+    <row r="13" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="29"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
+    </row>
+    <row r="14" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="29"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+    </row>
+    <row r="15" spans="1:14" s="13" customFormat="1" ht="10.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="37"/>
       <c r="B15" s="37"/>
       <c r="C15" s="37"/>
@@ -1035,49 +1044,49 @@
       <c r="F15" s="37"/>
       <c r="G15" s="37"/>
     </row>
-    <row r="16" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
+    <row r="16" spans="1:14" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
     </row>
     <row r="17" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
     </row>
     <row r="18" spans="1:7" s="13" customFormat="1" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-    </row>
-    <row r="19" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
     </row>
     <row r="20" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="38" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B20" s="38"/>
       <c r="C20" s="38"/>
@@ -1097,35 +1106,35 @@
     </row>
     <row r="22" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="E22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="F22" s="24" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="20"/>
       <c r="C23" s="25"/>
       <c r="D23" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="F23" s="7"/>
     </row>
     <row r="24" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C24" s="27"/>
       <c r="D24" s="8"/>
@@ -1134,7 +1143,7 @@
     </row>
     <row r="25" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C25" s="26"/>
       <c r="D25" s="10"/>
@@ -1454,28 +1463,24 @@
       <c r="F60" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="17">
     <mergeCell ref="A17:G17"/>
     <mergeCell ref="A18:G18"/>
     <mergeCell ref="A19:G19"/>
     <mergeCell ref="A20:G20"/>
     <mergeCell ref="A21:G21"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
     <mergeCell ref="A16:G16"/>
-    <mergeCell ref="A10:G10"/>
     <mergeCell ref="A7:G7"/>
     <mergeCell ref="A8:G8"/>
     <mergeCell ref="A9:G9"/>
     <mergeCell ref="A5:G5"/>
     <mergeCell ref="A6:G6"/>
-    <mergeCell ref="A11:G11"/>
-    <mergeCell ref="A12:G12"/>
-    <mergeCell ref="A13:G13"/>
-    <mergeCell ref="A14:G14"/>
     <mergeCell ref="A15:G15"/>
+    <mergeCell ref="A10:G14"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
   </mergeCells>
   <pageMargins left="0.82677165354330706" right="0.23622047244094488" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>